<commit_message>
update excel files, wl
</commit_message>
<xml_diff>
--- a/Registration_Summary.xlsx
+++ b/Registration_Summary.xlsx
@@ -443,16 +443,13 @@
         <x:v>0.2</x:v>
       </x:c>
       <x:c r="D2" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
-        <x:v>-9</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:7">
@@ -466,16 +463,13 @@
         <x:v>0.2</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
-        <x:v>-8</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
@@ -489,16 +483,13 @@
         <x:v>0.2</x:v>
       </x:c>
       <x:c r="D4" s="0" t="n">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="n">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="n">
-        <x:v>12</x:v>
-      </x:c>
       <x:c r="F4" s="0" t="n">
-        <x:v>-2</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:7">
@@ -512,16 +503,13 @@
         <x:v>0.2</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
-        <x:v>7</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>12</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F5" s="0" t="n">
-        <x:v>-5</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:7">
@@ -535,16 +523,13 @@
         <x:v>0.1</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
-        <x:v>14</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:7">
@@ -558,16 +543,13 @@
         <x:v>0.1</x:v>
       </x:c>
       <x:c r="D7" s="0" t="n">
-        <x:v>18</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
-        <x:v>6</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="F7" s="0" t="n">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>